<commit_message>
Revised code relationships tracker in prep for wind development.
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Foxhole Artillery Overlay Code Relationships.xlsx
+++ b/Assets/Scripts/Foxhole Artillery Overlay Code Relationships.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pamela\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pamela\Documents\GitHub\Foxhole Artillery Overlay\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6717C3-C128-4A29-A226-06C59FB48608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EBDEE8-4A93-48F6-B822-3A90897B7AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E2D7E774-1BE6-4F5B-B3C3-F3D3488B16FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E2D7E774-1BE6-4F5B-B3C3-F3D3488B16FE}"/>
   </bookViews>
   <sheets>
     <sheet name="GameObject Relationships" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="89">
   <si>
     <t>GameWindowCanvas</t>
   </si>
@@ -384,9 +384,6 @@
     </r>
   </si>
   <si>
-    <t>OptionsMenuPanel (WIP)</t>
-  </si>
-  <si>
     <t>CalculateAiming.cs</t>
   </si>
   <si>
@@ -409,6 +406,96 @@
   </si>
   <si>
     <t>WindGauge</t>
+  </si>
+  <si>
+    <t>WindGauge.increment_wind()</t>
+  </si>
+  <si>
+    <t>WindGauge.rotate_windgauge()</t>
+  </si>
+  <si>
+    <t>WindTierBackground</t>
+  </si>
+  <si>
+    <t>OpenMainPanel()</t>
+  </si>
+  <si>
+    <t>OpenOptionsPanel()</t>
+  </si>
+  <si>
+    <t>GridMarkerOpen()</t>
+  </si>
+  <si>
+    <t>GunMarkerOpen()</t>
+  </si>
+  <si>
+    <t>TargetMarkerOpen()</t>
+  </si>
+  <si>
+    <t>GetOffset()</t>
+  </si>
+  <si>
+    <t>MoveObject()</t>
+  </si>
+  <si>
+    <t>Awake()</t>
+  </si>
+  <si>
+    <t>increment_wind()</t>
+  </si>
+  <si>
+    <t>rotate_windgauge()</t>
+  </si>
+  <si>
+    <t>reset_wind_canvas()</t>
+  </si>
+  <si>
+    <t>Start()</t>
+  </si>
+  <si>
+    <t>reset_text()</t>
+  </si>
+  <si>
+    <t>reset_slider()</t>
+  </si>
+  <si>
+    <t>calculate_aimpoint()</t>
+  </si>
+  <si>
+    <t>draw_projectile_line()</t>
+  </si>
+  <si>
+    <t>get_scale()</t>
+  </si>
+  <si>
+    <t>get_wind()</t>
+  </si>
+  <si>
+    <t>scaleicon()</t>
+  </si>
+  <si>
+    <t>FixedUpdate()</t>
+  </si>
+  <si>
+    <t>OverUI()</t>
+  </si>
+  <si>
+    <t>CloseApp.cs</t>
+  </si>
+  <si>
+    <t>DropdownController.cs</t>
+  </si>
+  <si>
+    <t>populate_gunmodels()</t>
+  </si>
+  <si>
+    <t>get_gunplatform_selections()</t>
+  </si>
+  <si>
+    <t>reset_dropdowns()</t>
+  </si>
+  <si>
+    <t>ExitButton</t>
   </si>
   <si>
     <r>
@@ -420,6 +507,16 @@
         <charset val="2"/>
       </rPr>
       <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -430,80 +527,65 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>PointerClick</t>
-    </r>
-  </si>
-  <si>
-    <t>WindGauge.increment_wind()</t>
-  </si>
-  <si>
-    <t>WindGauge.rotate_windgauge()</t>
-  </si>
-  <si>
-    <t>WindTierBackground</t>
-  </si>
-  <si>
-    <t>OpenMainPanel()</t>
-  </si>
-  <si>
-    <t>OpenOptionsPanel()</t>
-  </si>
-  <si>
-    <t>GridMarkerOpen()</t>
-  </si>
-  <si>
-    <t>GunMarkerOpen()</t>
-  </si>
-  <si>
-    <t>TargetMarkerOpen()</t>
-  </si>
-  <si>
-    <t>GetOffset()</t>
-  </si>
-  <si>
-    <t>MoveObject()</t>
-  </si>
-  <si>
-    <t>Awake()</t>
-  </si>
-  <si>
-    <t>increment_wind()</t>
-  </si>
-  <si>
-    <t>rotate_windgauge()</t>
-  </si>
-  <si>
-    <t>reset_wind_canvas()</t>
-  </si>
-  <si>
-    <t>Start()</t>
-  </si>
-  <si>
-    <t>reset_text()</t>
-  </si>
-  <si>
-    <t>reset_slider()</t>
-  </si>
-  <si>
-    <t>calculate_aimpoint()</t>
-  </si>
-  <si>
-    <t>draw_projectile_line()</t>
-  </si>
-  <si>
-    <t>get_scale()</t>
-  </si>
-  <si>
-    <t>get_wind()</t>
-  </si>
-  <si>
-    <t>scaleicon()</t>
-  </si>
-  <si>
-    <t>FixedUpdate()</t>
-  </si>
-  <si>
-    <t>OverUI()</t>
+      <t>On Click</t>
+    </r>
+  </si>
+  <si>
+    <t>CloseApp.close_app()</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>WeaponTypeDropdown</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OnValueChanged (Int32)</t>
+    </r>
+  </si>
+  <si>
+    <t>DropdownController.populate_gunmodels()</t>
+  </si>
+  <si>
+    <t>OptionsMenuPanel</t>
+  </si>
+  <si>
+    <t>WeaponDropdown</t>
+  </si>
+  <si>
+    <t>DropdownController.get_gunplatform_selections()</t>
+  </si>
+  <si>
+    <t>WindTierInteract</t>
   </si>
 </sst>
 </file>
@@ -605,17 +687,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,19 +1017,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55930E3-C8DA-4BD4-AC96-94C294597FC7}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1000,7 +1087,7 @@
       <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E8" t="s">
@@ -1014,7 +1101,7 @@
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D9" t="s">
@@ -1028,7 +1115,7 @@
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D10" t="s">
@@ -1042,7 +1129,7 @@
       <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D11" t="s">
@@ -1059,7 +1146,7 @@
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1089,7 +1176,7 @@
       <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D16" t="s">
@@ -1103,7 +1190,7 @@
       <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D17" t="s">
@@ -1117,7 +1204,7 @@
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
@@ -1156,7 +1243,7 @@
       <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D22" t="s">
@@ -1170,7 +1257,7 @@
       <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D23" t="s">
@@ -1184,7 +1271,7 @@
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D24" t="s">
@@ -1208,8 +1295,8 @@
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>9</v>
+      <c r="B28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1219,36 +1306,35 @@
       <c r="B29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
+      <c r="C29" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" t="s">
-        <v>27</v>
+      <c r="B32" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1258,33 +1344,25 @@
       <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" t="s">
-        <v>31</v>
+      <c r="C33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" t="s">
-        <v>28</v>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1294,14 +1372,8 @@
       <c r="B36" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" t="s">
-        <v>32</v>
+      <c r="C36" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1311,6 +1383,15 @@
       <c r="B37" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
@@ -1319,9 +1400,6 @@
       <c r="B38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C38" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
@@ -1330,14 +1408,8 @@
       <c r="B39" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39" t="s">
-        <v>33</v>
+      <c r="C39" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1347,6 +1419,15 @@
       <c r="B40" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
@@ -1355,9 +1436,6 @@
       <c r="B41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
@@ -1366,50 +1444,79 @@
       <c r="B42" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="B43" s="1"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
+    <row r="47" spans="1:5">
+      <c r="B47" s="1"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="B45" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B48" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B49" t="s">
-        <v>11</v>
+      <c r="B49" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1417,7 +1524,7 @@
         <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1428,7 +1535,7 @@
         <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1439,7 +1546,7 @@
         <v>23</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1449,8 +1556,14 @@
       <c r="B53" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C53" t="s">
-        <v>44</v>
+      <c r="C53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1460,15 +1573,6 @@
       <c r="B54" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E54" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
@@ -1477,8 +1581,9 @@
       <c r="B55" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="6"/>
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
@@ -1487,69 +1592,43 @@
       <c r="B56" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C56" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E57" t="s">
-        <v>51</v>
+      <c r="C56" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>23</v>
+      <c r="A58" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" t="s">
-        <v>46</v>
+      <c r="B59" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E60" t="s">
-        <v>51</v>
+      <c r="B60" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>23</v>
+      <c r="B61" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1560,7 +1639,7 @@
         <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1570,13 +1649,7 @@
       <c r="B63" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="C63" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1587,6 +1660,9 @@
       <c r="B64" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C64" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
@@ -1596,7 +1672,7 @@
         <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1606,14 +1682,8 @@
       <c r="B66" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E66" t="s">
-        <v>51</v>
+      <c r="C66" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1623,6 +1693,9 @@
       <c r="B67" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C67" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
@@ -1632,7 +1705,7 @@
         <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1642,14 +1715,8 @@
       <c r="B69" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E69" t="s">
-        <v>52</v>
+      <c r="C69" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1662,20 +1729,90 @@
       <c r="C70" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E70" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" t="s">
+      <c r="A72" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E74" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
-      <c r="B73" t="s">
+    <row r="78" spans="1:5">
+      <c r="B78" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1687,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A03FFF-E266-42E1-9B91-A42D6D23388B}">
-  <dimension ref="A2:B34"/>
+  <dimension ref="A2:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1700,7 +1837,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1709,7 +1846,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1717,7 +1854,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1725,7 +1862,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1733,7 +1870,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1741,11 +1878,11 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1754,7 +1891,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1762,12 +1899,12 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
-        <v>43</v>
+      <c r="A13" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1775,7 +1912,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1783,7 +1920,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1791,7 +1928,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1799,12 +1936,12 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="7" t="s">
-        <v>42</v>
+      <c r="A19" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1812,7 +1949,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1820,7 +1957,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1828,7 +1965,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1836,7 +1973,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1844,7 +1981,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1852,7 +1989,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1860,11 +1997,11 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1873,11 +2010,11 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1886,7 +2023,7 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1894,7 +2031,7 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1902,10 +2039,58 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="7" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added in the ability to toggle between small and large scale grids. Updated Excel list of functions and Unity object heirarchy. Tweaked grid scale slider bar min/max values to make it easier to use at larger numbers.
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Foxhole Artillery Overlay Code Relationships.xlsx
+++ b/Assets/Scripts/Foxhole Artillery Overlay Code Relationships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pamela\Documents\GitHub\Foxhole Artillery Overlay\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B3F33C-CF4B-49C8-AA6C-365731D3054D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E447D-21DF-453A-A53E-0F205DBAEA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E2D7E774-1BE6-4F5B-B3C3-F3D3488B16FE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{E2D7E774-1BE6-4F5B-B3C3-F3D3488B16FE}"/>
   </bookViews>
   <sheets>
     <sheet name="GameObject Relationships" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="127">
   <si>
     <t>GameWindowCanvas</t>
   </si>
@@ -601,6 +601,153 @@
       </rPr>
       <t>PointerUp</t>
     </r>
+  </si>
+  <si>
+    <t>DispersionCircleIcon</t>
+  </si>
+  <si>
+    <t>MarkerLocations.cs</t>
+  </si>
+  <si>
+    <t>HideIconsButton</t>
+  </si>
+  <si>
+    <t>Visibility.cs</t>
+  </si>
+  <si>
+    <t>Visibility.ChangeVis()</t>
+  </si>
+  <si>
+    <t>GridChanger.cs</t>
+  </si>
+  <si>
+    <t>ToggleGroup</t>
+  </si>
+  <si>
+    <t>SmallToggle</t>
+  </si>
+  <si>
+    <t>LargeToggle</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OnValueChanged (Boolean)</t>
+    </r>
+  </si>
+  <si>
+    <t>ChangeVis()</t>
+  </si>
+  <si>
+    <t>visReset()</t>
+  </si>
+  <si>
+    <t>MoveUIObjectTarget.cs</t>
+  </si>
+  <si>
+    <t>OpenHelpMenu()</t>
+  </si>
+  <si>
+    <t>ChangeGrid()</t>
+  </si>
+  <si>
+    <t>get_gun_marker_position()</t>
+  </si>
+  <si>
+    <t>get_target_marker_position()</t>
+  </si>
+  <si>
+    <t>get_dispersion_marker_position()</t>
+  </si>
+  <si>
+    <t>get_aimline_position()</t>
+  </si>
+  <si>
+    <t>get_aimline_up_transform()</t>
+  </si>
+  <si>
+    <t>get_grid_marker_scale()</t>
+  </si>
+  <si>
+    <t>set_gun_marker_position()</t>
+  </si>
+  <si>
+    <t>set_target_marker_position()</t>
+  </si>
+  <si>
+    <t>set_dispersion_marker_position()</t>
+  </si>
+  <si>
+    <t>set_grid_marker_position()</t>
+  </si>
+  <si>
+    <t>set_aimline_position()</t>
+  </si>
+  <si>
+    <t>set_dispersion_marker_scale()</t>
+  </si>
+  <si>
+    <t>set_grid_marker_scale()</t>
+  </si>
+  <si>
+    <t>rotate_aimline_panel()</t>
+  </si>
+  <si>
+    <t>set_aimline_panel_length()</t>
+  </si>
+  <si>
+    <t>is_gun_marker_open()</t>
+  </si>
+  <si>
+    <t>is_target_marker_open()</t>
+  </si>
+  <si>
+    <t>is_grid_marker_open()</t>
+  </si>
+  <si>
+    <t>set_gun_marker_open()</t>
+  </si>
+  <si>
+    <t>set_target_marker_open()</t>
+  </si>
+  <si>
+    <t>set_dispersion_marker_open()</t>
+  </si>
+  <si>
+    <t>set_grid_marker_open()</t>
+  </si>
+  <si>
+    <t>set_aimline_open()</t>
+  </si>
+  <si>
+    <t>reset_slider()</t>
   </si>
 </sst>
 </file>
@@ -723,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -732,14 +879,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55930E3-C8DA-4BD4-AC96-94C294597FC7}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,19 +1242,16 @@
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>82</v>
+      <c r="B5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1111,7 +1262,7 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1122,7 +1273,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1132,14 +1283,8 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
+      <c r="C9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1149,11 +1294,14 @@
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1164,10 +1312,10 @@
         <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1177,72 +1325,60 @@
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>87</v>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
+      <c r="B16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1252,25 +1388,36 @@
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
+      <c r="C19" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>84</v>
+      <c r="B21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1280,36 +1427,24 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
-        <v>12</v>
+      <c r="C22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
+      <c r="B24" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1319,70 +1454,82 @@
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>1</v>
+      <c r="A27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" t="s">
-        <v>71</v>
+      <c r="B28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>66</v>
+      <c r="A30" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>73</v>
+      <c r="B31" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>6</v>
+      <c r="B33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1396,21 +1543,20 @@
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
+      <c r="B36" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1421,7 +1567,7 @@
         <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1431,33 +1577,24 @@
       <c r="B38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" t="s">
-        <v>27</v>
+      <c r="C38" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" t="s">
-        <v>24</v>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1467,33 +1604,25 @@
       <c r="B41" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41" t="s">
-        <v>28</v>
+      <c r="C41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" t="s">
-        <v>25</v>
+      <c r="B43" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1503,14 +1632,8 @@
       <c r="B44" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" t="s">
-        <v>29</v>
+      <c r="C44" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1520,6 +1643,15 @@
       <c r="B45" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
@@ -1528,9 +1660,6 @@
       <c r="B46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C46" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
@@ -1539,40 +1668,61 @@
       <c r="B47" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="2"/>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>2</v>
+      <c r="A49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>67</v>
+      <c r="B50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B51" t="s">
-        <v>78</v>
+      <c r="B51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1582,9 +1732,6 @@
       <c r="B52" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C52" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
@@ -1594,7 +1741,7 @@
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1607,76 +1754,84 @@
       <c r="C54" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>76</v>
+      <c r="D54" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="E54" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" t="s">
-        <v>79</v>
+      <c r="A56" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E57" t="s">
-        <v>80</v>
+      <c r="B57" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>3</v>
+      <c r="A59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B60" t="s">
-        <v>37</v>
+      <c r="B60" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B61" t="s">
-        <v>8</v>
+      <c r="B61" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B62" t="s">
-        <v>9</v>
+      <c r="B62" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1686,9 +1841,6 @@
       <c r="B63" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C63" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
@@ -1698,7 +1850,7 @@
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1708,8 +1860,14 @@
       <c r="B65" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C65" t="s">
-        <v>39</v>
+      <c r="C65" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E65" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1719,9 +1877,8 @@
       <c r="B66" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C66" t="s">
-        <v>40</v>
-      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
@@ -1730,8 +1887,8 @@
       <c r="B67" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C67" t="s">
-        <v>41</v>
+      <c r="C67" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1741,8 +1898,11 @@
       <c r="B68" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C68" t="s">
-        <v>42</v>
+      <c r="C68" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D68" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1752,8 +1912,14 @@
       <c r="B69" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C69" t="s">
-        <v>43</v>
+      <c r="C69" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1763,8 +1929,8 @@
       <c r="B70" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C70" t="s">
-        <v>81</v>
+      <c r="C70" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1777,11 +1943,8 @@
       <c r="C71" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E71" t="s">
-        <v>45</v>
+      <c r="D71" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1794,73 +1957,227 @@
       <c r="C72" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" t="s">
-        <v>20</v>
+      <c r="D72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C74" t="s">
-        <v>44</v>
+      <c r="A74" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E75" t="s">
-        <v>46</v>
+      <c r="B75" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E86" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E87" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
-      <c r="A78" t="s">
+    <row r="88" spans="1:5">
+      <c r="A88" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E90" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="B79" t="s">
+    <row r="94" spans="1:5">
+      <c r="B94" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1872,25 +2189,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A03FFF-E266-42E1-9B91-A42D6D23388B}">
-  <dimension ref="A2:B41"/>
+  <dimension ref="A2:B82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
@@ -1898,7 +2215,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
@@ -1906,7 +2223,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
@@ -1914,7 +2231,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
@@ -1922,7 +2239,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
@@ -1930,12 +2247,12 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
@@ -1943,7 +2260,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
@@ -1951,12 +2268,12 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
@@ -1964,7 +2281,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
@@ -1972,7 +2289,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
@@ -1980,7 +2297,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
@@ -1988,12 +2305,12 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -2001,7 +2318,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -2009,7 +2326,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B22" t="s">
@@ -2017,7 +2334,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B23" t="s">
@@ -2025,7 +2342,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B24" t="s">
@@ -2033,12 +2350,12 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B27" t="s">
@@ -2046,12 +2363,12 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B30" t="s">
@@ -2059,7 +2376,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B31" t="s">
@@ -2067,7 +2384,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B32" t="s">
@@ -2075,12 +2392,12 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B35" t="s">
@@ -2088,7 +2405,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B36" t="s">
@@ -2096,7 +2413,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B37" t="s">
@@ -2104,7 +2421,7 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B38" t="s">
@@ -2112,16 +2429,306 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B41" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="9"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="9"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>